<commit_message>
Modifying Sets-IEMM.xlsx and LMADefs-IEMM.xls to add hydrogen to reports
</commit_message>
<xml_diff>
--- a/Sets-IEMM.xlsx
+++ b/Sets-IEMM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IEMM\IEMM_MIG\IEMM_V58_10-1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda_models\IEMM_v60_10-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0687BAF4-B5D2-4A13-9651-FB90E352799A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B70F88E9-4C73-4845-BF68-E9C86EA1C9A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TechSup" sheetId="4" r:id="rId1"/>
@@ -25,12 +25,59 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'EFD classification'!$H$3:$J$78</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TechSup!$F$3:$G$61</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Mahmoud Mobir</author>
+  </authors>
+  <commentList>
+    <comment ref="B69" authorId="0" shapeId="0" xr:uid="{E699EE90-56D9-4886-9B92-A6BC016AB6E6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mahmoud Mobir:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+12-6-2021
+added to track hydrogen production
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="303">
   <si>
     <t>Pset_CI</t>
   </si>
@@ -822,13 +869,130 @@
   </si>
   <si>
     <t>Storage</t>
+  </si>
+  <si>
+    <t>S_H2P</t>
+  </si>
+  <si>
+    <t>S_H2P-All</t>
+  </si>
+  <si>
+    <t>PRE</t>
+  </si>
+  <si>
+    <t>S*H2*,ELCH2*</t>
+  </si>
+  <si>
+    <t>H2 prod-all</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H2 prod </t>
+  </si>
+  <si>
+    <t>H2 prod (CCS)</t>
+  </si>
+  <si>
+    <t>H2 Prod Bio-all</t>
+  </si>
+  <si>
+    <t>H2 Prod Biomass</t>
+  </si>
+  <si>
+    <t>H2 Prod Biomass CCS</t>
+  </si>
+  <si>
+    <t>H2 Prod Coa-all</t>
+  </si>
+  <si>
+    <t>H2 Prod Coal</t>
+  </si>
+  <si>
+    <t>H2 Prod Coal CCS</t>
+  </si>
+  <si>
+    <t>H2 Prod Electricity</t>
+  </si>
+  <si>
+    <t>H2 Prod Gas-all</t>
+  </si>
+  <si>
+    <t>H2 Prod Gas</t>
+  </si>
+  <si>
+    <t>H2 Prod Gas CCS</t>
+  </si>
+  <si>
+    <t>H2 Prod Oil</t>
+  </si>
+  <si>
+    <t>H2 Prod Nuclear</t>
+  </si>
+  <si>
+    <t>S_H2P_BIO-All</t>
+  </si>
+  <si>
+    <t>S_H2P_BIO</t>
+  </si>
+  <si>
+    <t>S_H2P_BIO-CCS</t>
+  </si>
+  <si>
+    <t>S_H2P_COA-All</t>
+  </si>
+  <si>
+    <t>S_H2P_COA</t>
+  </si>
+  <si>
+    <t>S_H2P_COA-CCS</t>
+  </si>
+  <si>
+    <t>S_H2P_ELC</t>
+  </si>
+  <si>
+    <t>S_H2P_GAS-All</t>
+  </si>
+  <si>
+    <t>S_H2P_GAS</t>
+  </si>
+  <si>
+    <t>S_H2P_GAS-CCS</t>
+  </si>
+  <si>
+    <t>S_H2P_OIL</t>
+  </si>
+  <si>
+    <t>S_H2P_NUC</t>
+  </si>
+  <si>
+    <t>SHFO*H2*</t>
+  </si>
+  <si>
+    <t>ENUCH2*</t>
+  </si>
+  <si>
+    <t>ELC*,-BIO*,-COA*,-GAS*</t>
+  </si>
+  <si>
+    <t>SGAS*H2*</t>
+  </si>
+  <si>
+    <t>*ELCH2*</t>
+  </si>
+  <si>
+    <t>SYNH2*</t>
+  </si>
+  <si>
+    <t>TRNH2</t>
+  </si>
+  <si>
+    <t>Hydrogen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -885,6 +1049,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1290,36 +1467,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="B2:J68"/>
+  <dimension ref="B2:J83"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B70" sqref="B70:H83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="8"/>
-    <col min="2" max="2" width="21.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" style="8"/>
+    <col min="2" max="2" width="21.7265625" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.453125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.7265625" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.26953125" style="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="77.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="8"/>
+    <col min="9" max="9" width="12.54296875" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="77.7265625" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.1796875" style="8"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B2" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="9" t="s">
         <v>2</v>
       </c>
@@ -1348,7 +1525,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B4" s="8" t="s">
         <v>41</v>
       </c>
@@ -1365,7 +1542,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
       <c r="C5" s="8" t="s">
         <v>49</v>
       </c>
@@ -1379,7 +1556,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B6" s="8" t="s">
         <v>247</v>
       </c>
@@ -1395,7 +1572,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B7" s="8" t="s">
         <v>248</v>
       </c>
@@ -1411,7 +1588,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B8" s="8" t="s">
         <v>126</v>
       </c>
@@ -1426,7 +1603,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B9" s="8" t="s">
         <v>224</v>
       </c>
@@ -1441,7 +1618,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B10" s="8" t="s">
         <v>126</v>
       </c>
@@ -1456,7 +1633,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B11" s="8" t="s">
         <v>224</v>
       </c>
@@ -1472,7 +1649,7 @@
         <v>natural-gas</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B12" s="8" t="s">
         <v>247</v>
       </c>
@@ -1489,7 +1666,7 @@
       </c>
       <c r="I12" s="12"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B13" s="8" t="s">
         <v>248</v>
       </c>
@@ -1506,7 +1683,7 @@
       </c>
       <c r="I13" s="12"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B14" s="8" t="s">
         <v>246</v>
       </c>
@@ -1527,7 +1704,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B15" s="8" t="s">
         <v>126</v>
       </c>
@@ -1542,7 +1719,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B16" s="8" t="s">
         <v>224</v>
       </c>
@@ -1557,7 +1734,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B17" s="8" t="s">
         <v>126</v>
       </c>
@@ -1572,7 +1749,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B18" s="8" t="s">
         <v>126</v>
       </c>
@@ -1586,7 +1763,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B19" s="8" t="s">
         <v>224</v>
       </c>
@@ -1601,7 +1778,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B20" s="8" t="s">
         <v>224</v>
       </c>
@@ -1616,7 +1793,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B21" s="8" t="s">
         <v>126</v>
       </c>
@@ -1630,7 +1807,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B22" s="8" t="s">
         <v>224</v>
       </c>
@@ -1644,7 +1821,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B23" s="8" t="s">
         <v>246</v>
       </c>
@@ -1659,7 +1836,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B24" s="8" t="s">
         <v>126</v>
       </c>
@@ -1674,7 +1851,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B25" s="8" t="s">
         <v>224</v>
       </c>
@@ -1689,7 +1866,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B26" s="8" t="s">
         <v>246</v>
       </c>
@@ -1704,7 +1881,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B27" s="8" t="s">
         <v>28</v>
       </c>
@@ -1721,7 +1898,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B28" s="8" t="s">
         <v>28</v>
       </c>
@@ -1741,7 +1918,7 @@
         <v>ELEBIO-O</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B29" s="8" t="s">
         <v>28</v>
       </c>
@@ -1757,11 +1934,11 @@
         <v>ELECOA-O</v>
       </c>
       <c r="H29" s="8" t="str">
-        <f t="shared" ref="H29:H68" si="0">G29</f>
+        <f t="shared" ref="H29:H70" si="0">G29</f>
         <v>ELECOA-O</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B30" s="8" t="s">
         <v>28</v>
       </c>
@@ -1781,7 +1958,7 @@
         <v>ELEGAS-O</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B31" s="8" t="s">
         <v>28</v>
       </c>
@@ -1801,7 +1978,7 @@
         <v>ELEGEO-O</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B32" s="8" t="s">
         <v>28</v>
       </c>
@@ -1821,7 +1998,7 @@
         <v>ELEHYD-O</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B33" s="8" t="s">
         <v>28</v>
       </c>
@@ -1841,7 +2018,7 @@
         <v>ELENUC-O</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B34" s="8" t="s">
         <v>28</v>
       </c>
@@ -1861,7 +2038,7 @@
         <v>ELEOIL-O</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B35" s="8" t="s">
         <v>28</v>
       </c>
@@ -1880,7 +2057,7 @@
         <v>ELEDST-O</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B36" s="8" t="s">
         <v>28</v>
       </c>
@@ -1900,7 +2077,7 @@
         <v>ELESOL-O</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B37" s="8" t="s">
         <v>28</v>
       </c>
@@ -1920,7 +2097,7 @@
         <v>ELEWAS-O</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B38" s="8" t="s">
         <v>28</v>
       </c>
@@ -1940,7 +2117,7 @@
         <v>ELEWIN-O</v>
       </c>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B39" s="8" t="s">
         <v>246</v>
       </c>
@@ -1960,7 +2137,7 @@
         <v>ELEBIO-N</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B40" s="8" t="s">
         <v>28</v>
       </c>
@@ -1980,7 +2157,7 @@
         <v>ELECOA-N</v>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B41" s="8" t="s">
         <v>28</v>
       </c>
@@ -2000,7 +2177,7 @@
         <v>ELEGAS-N</v>
       </c>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B42" s="8" t="s">
         <v>246</v>
       </c>
@@ -2020,7 +2197,7 @@
         <v>ELEGEO-N</v>
       </c>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B43" s="8" t="s">
         <v>246</v>
       </c>
@@ -2040,7 +2217,7 @@
         <v>ELEHYD-N</v>
       </c>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B44" s="8" t="s">
         <v>28</v>
       </c>
@@ -2060,7 +2237,7 @@
         <v>ELENUC-N</v>
       </c>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B45" s="8" t="s">
         <v>28</v>
       </c>
@@ -2080,7 +2257,7 @@
         <v>ELEOIL-N</v>
       </c>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B46" s="8" t="s">
         <v>28</v>
       </c>
@@ -2099,7 +2276,7 @@
         <v>ELEDST-N</v>
       </c>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B47" s="8" t="s">
         <v>246</v>
       </c>
@@ -2119,7 +2296,7 @@
         <v>ELESOL-N</v>
       </c>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B48" s="8" t="s">
         <v>28</v>
       </c>
@@ -2139,7 +2316,7 @@
         <v>ELEWAS-N</v>
       </c>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B49" s="8" t="s">
         <v>246</v>
       </c>
@@ -2159,7 +2336,7 @@
         <v>ELEWIN-N</v>
       </c>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B50" s="12" t="s">
         <v>126</v>
       </c>
@@ -2180,7 +2357,7 @@
         <v>ELECOA-S</v>
       </c>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B51" s="12" t="s">
         <v>126</v>
       </c>
@@ -2202,7 +2379,7 @@
         <v>ELEGAS-S</v>
       </c>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B52" s="12" t="s">
         <v>126</v>
       </c>
@@ -2224,7 +2401,7 @@
         <v>ELEBIO-S</v>
       </c>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B53" s="12" t="s">
         <v>126</v>
       </c>
@@ -2244,7 +2421,7 @@
         <v>ELECOA-NS</v>
       </c>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B54" s="12" t="s">
         <v>126</v>
       </c>
@@ -2267,7 +2444,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B55" s="12" t="s">
         <v>126</v>
       </c>
@@ -2287,7 +2464,7 @@
         <v>ELEBIO-NS</v>
       </c>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B56" s="8" t="s">
         <v>126</v>
       </c>
@@ -2305,7 +2482,7 @@
         <v>EGasOil_N-CT</v>
       </c>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B57" s="8" t="s">
         <v>126</v>
       </c>
@@ -2323,7 +2500,7 @@
         <v>EGasOil_N-CC</v>
       </c>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B58" s="8" t="s">
         <v>126</v>
       </c>
@@ -2341,7 +2518,7 @@
         <v>EGasOil_N-ST</v>
       </c>
     </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B59" s="8" t="s">
         <v>126</v>
       </c>
@@ -2359,7 +2536,7 @@
         <v>EGasOil_E-CT</v>
       </c>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B60" s="8" t="s">
         <v>126</v>
       </c>
@@ -2377,7 +2554,7 @@
         <v>EGasOil_E-CC</v>
       </c>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B61" s="8" t="s">
         <v>126</v>
       </c>
@@ -2395,7 +2572,7 @@
         <v>EGasOil_E-ST</v>
       </c>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.35">
       <c r="C62" s="8" t="s">
         <v>244</v>
       </c>
@@ -2407,7 +2584,7 @@
         <v>ERETargDum</v>
       </c>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B63" s="8" t="s">
         <v>79</v>
       </c>
@@ -2421,7 +2598,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B64" s="8" t="s">
         <v>126</v>
       </c>
@@ -2439,7 +2616,7 @@
         <v>ECoal_E-CC</v>
       </c>
     </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B65" s="8" t="s">
         <v>126</v>
       </c>
@@ -2461,7 +2638,7 @@
         <v>ECoal_N-CC</v>
       </c>
     </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B66" s="8" t="s">
         <v>126</v>
       </c>
@@ -2483,7 +2660,7 @@
         <v>ECoal_N-CS</v>
       </c>
     </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B67" s="8" t="s">
         <v>126</v>
       </c>
@@ -2501,7 +2678,7 @@
         <v>ECoal_N-ST</v>
       </c>
     </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B68" s="8" t="s">
         <v>126</v>
       </c>
@@ -2517,36 +2694,252 @@
       <c r="H68" s="8" t="str">
         <f t="shared" si="0"/>
         <v>ECoal_E-ST</v>
+      </c>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B69" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="C69" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="G69" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="H69" s="8" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B70" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="F70" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="G70" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="H70" s="8" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B71" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="F71" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="G71" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="H71" s="8" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B72" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="E72" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G72" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="H72" s="8" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B73" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="F73" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="G73" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="H73" s="8" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B74" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="F74" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="G74" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="H74" s="8" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B75" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="E75" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G75" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="H75" s="8" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B76" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="F76" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="G76" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="H76" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B77" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="F77" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="G77" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="H77" s="8" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B78" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="C78" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="E78" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="G78" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="H78" s="8" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B79" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="C79" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="E79" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G79" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="H79" s="8" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B80" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="F80" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="G80" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="H80" s="8" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="81" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B81" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="F81" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="G81" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="H81" s="8" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B82" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="C82" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="G82" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="H82" s="8" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C83" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="G83" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="H83" s="8" t="s">
+        <v>282</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="B2:G10"/>
+  <dimension ref="B2:G11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="54.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
@@ -2566,7 +2959,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>11</v>
       </c>
@@ -2583,7 +2976,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>11</v>
       </c>
@@ -2600,7 +2993,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>11</v>
       </c>
@@ -2617,7 +3010,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>11</v>
       </c>
@@ -2634,7 +3027,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>11</v>
       </c>
@@ -2651,7 +3044,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>11</v>
       </c>
@@ -2668,7 +3061,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>11</v>
       </c>
@@ -2683,6 +3076,20 @@
       </c>
       <c r="G10" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>300</v>
+      </c>
+      <c r="E11" t="s">
+        <v>301</v>
+      </c>
+      <c r="F11" t="s">
+        <v>302</v>
       </c>
     </row>
   </sheetData>
@@ -2695,26 +3102,26 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B2:O58"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.81640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="34.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -2749,7 +3156,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>126</v>
       </c>
@@ -2772,7 +3179,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B5" s="5" t="s">
         <v>126</v>
       </c>
@@ -2795,7 +3202,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B6" s="5" t="s">
         <v>126</v>
       </c>
@@ -2818,7 +3225,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B7" s="5" t="s">
         <v>126</v>
       </c>
@@ -2841,7 +3248,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B8" s="5" t="s">
         <v>126</v>
       </c>
@@ -2864,7 +3271,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B9" s="5" t="s">
         <v>126</v>
       </c>
@@ -2887,7 +3294,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B10" s="5" t="s">
         <v>126</v>
       </c>
@@ -2910,7 +3317,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B11" s="5" t="s">
         <v>126</v>
       </c>
@@ -2933,7 +3340,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="2:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:15" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B12" s="5" t="s">
         <v>126</v>
       </c>
@@ -2964,7 +3371,7 @@
       </c>
       <c r="O12"/>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B13" s="5" t="s">
         <v>126</v>
       </c>
@@ -2987,7 +3394,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B14" s="5" t="s">
         <v>126</v>
       </c>
@@ -3010,7 +3417,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B15" s="5" t="s">
         <v>126</v>
       </c>
@@ -3033,7 +3440,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B16" s="5" t="s">
         <v>126</v>
       </c>
@@ -3056,7 +3463,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B17" s="5" t="s">
         <v>126</v>
       </c>
@@ -3079,7 +3486,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="2:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B18" s="5" t="s">
         <v>126</v>
       </c>
@@ -3109,7 +3516,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B19" s="5" t="s">
         <v>126</v>
       </c>
@@ -3132,7 +3539,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B20" s="5" t="s">
         <v>126</v>
       </c>
@@ -3155,7 +3562,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B21" s="5" t="s">
         <v>126</v>
       </c>
@@ -3178,7 +3585,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="22" spans="2:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B22" s="5" t="s">
         <v>126</v>
       </c>
@@ -3208,7 +3615,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B23" s="5" t="s">
         <v>126</v>
       </c>
@@ -3231,7 +3638,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B24" s="5" t="s">
         <v>126</v>
       </c>
@@ -3254,7 +3661,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B25" s="5" t="s">
         <v>126</v>
       </c>
@@ -3277,7 +3684,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B26" s="5" t="s">
         <v>126</v>
       </c>
@@ -3300,7 +3707,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B27" s="5" t="s">
         <v>126</v>
       </c>
@@ -3323,7 +3730,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B28" s="5" t="s">
         <v>126</v>
       </c>
@@ -3346,7 +3753,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B29" s="5" t="s">
         <v>126</v>
       </c>
@@ -3369,7 +3776,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B30" s="5" t="s">
         <v>126</v>
       </c>
@@ -3392,7 +3799,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B31" s="5" t="s">
         <v>126</v>
       </c>
@@ -3415,7 +3822,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B32" s="5" t="s">
         <v>126</v>
       </c>
@@ -3438,7 +3845,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B33" s="5" t="s">
         <v>126</v>
       </c>
@@ -3461,7 +3868,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B34" s="5" t="s">
         <v>126</v>
       </c>
@@ -3484,7 +3891,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B35" s="5" t="s">
         <v>126</v>
       </c>
@@ -3507,7 +3914,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="37" spans="2:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B37"/>
       <c r="C37"/>
       <c r="D37"/>
@@ -3522,7 +3929,7 @@
       <c r="M37"/>
       <c r="N37"/>
     </row>
-    <row r="44" spans="2:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B44"/>
       <c r="C44"/>
       <c r="D44"/>
@@ -3537,7 +3944,7 @@
       <c r="M44"/>
       <c r="N44"/>
     </row>
-    <row r="48" spans="2:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B48"/>
       <c r="C48"/>
       <c r="D48"/>
@@ -3552,7 +3959,7 @@
       <c r="M48"/>
       <c r="N48"/>
     </row>
-    <row r="51" spans="2:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B51"/>
       <c r="C51"/>
       <c r="D51"/>
@@ -3567,7 +3974,7 @@
       <c r="M51"/>
       <c r="N51"/>
     </row>
-    <row r="58" spans="2:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B58"/>
       <c r="C58"/>
       <c r="D58"/>
@@ -3594,14 +4001,14 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -3641,26 +4048,26 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="6"/>
+    <col min="1" max="2" width="9.1796875" style="6"/>
     <col min="3" max="3" width="12" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="6"/>
-    <col min="8" max="8" width="8.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="4" width="8.26953125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.54296875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.453125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1796875" style="6"/>
+    <col min="8" max="8" width="8.7265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.453125" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.1796875" style="6"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B2" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
@@ -3689,7 +4096,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
       <c r="C4" s="6" t="s">
         <v>151</v>
       </c>
@@ -3701,7 +4108,7 @@
         <v>GridLev1</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
       <c r="C5" s="6" t="s">
         <v>152</v>
       </c>
@@ -3713,7 +4120,7 @@
         <v>GridLev2</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
       <c r="C6" s="6" t="s">
         <v>153</v>
       </c>
@@ -3725,7 +4132,7 @@
         <v>GridLev3</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
       <c r="C7" s="8" t="s">
         <v>177</v>
       </c>
@@ -3739,7 +4146,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
       <c r="C8" s="5" t="s">
         <v>180</v>
       </c>
@@ -3765,32 +4172,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B2:M35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="6"/>
-    <col min="3" max="3" width="15.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="9.140625" style="6"/>
-    <col min="13" max="13" width="4.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="2" width="9.1796875" style="6"/>
+    <col min="3" max="3" width="15.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.26953125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.453125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.54296875" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.453125" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="9.1796875" style="6"/>
+    <col min="13" max="13" width="4.1796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.1796875" style="6"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B2" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
@@ -3819,7 +4226,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C4" s="6" t="str">
         <f>"*[_]"&amp;M4&amp;"[_]*"</f>
         <v>*[_]C01[_]*</v>
@@ -3839,7 +4246,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C5" s="6" t="str">
         <f t="shared" ref="C5:C13" si="0">"*[_]"&amp;M5&amp;"[_]*"</f>
         <v>*[_]C02[_]*</v>
@@ -3859,7 +4266,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C6" s="6" t="str">
         <f t="shared" si="0"/>
         <v>*[_]C03[_]*</v>
@@ -3879,7 +4286,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C7" s="6" t="str">
         <f t="shared" si="0"/>
         <v>*[_]C04[_]*</v>
@@ -3899,7 +4306,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C8" s="6" t="str">
         <f t="shared" si="0"/>
         <v>*[_]C05[_]*</v>
@@ -3919,7 +4326,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C9" s="6" t="str">
         <f t="shared" si="0"/>
         <v>*[_]C06[_]*</v>
@@ -3939,7 +4346,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C10" s="6" t="str">
         <f t="shared" si="0"/>
         <v>*[_]C07[_]*</v>
@@ -3959,7 +4366,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C11" s="6" t="str">
         <f t="shared" si="0"/>
         <v>*[_]C08[_]*</v>
@@ -3979,7 +4386,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C12" s="6" t="str">
         <f t="shared" si="0"/>
         <v>*[_]C09[_]*</v>
@@ -3999,7 +4406,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C13" s="6" t="str">
         <f t="shared" si="0"/>
         <v>*[_]C10[_]*</v>
@@ -4019,7 +4426,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C14" s="8" t="str">
         <f>"*WON*[_]"&amp;M14&amp;"[_]*"</f>
         <v>*WON*[_]C1[_]*</v>
@@ -4039,7 +4446,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C15" s="8" t="str">
         <f t="shared" ref="C15:C22" si="3">"*WON*[_]"&amp;M15&amp;"[_]*"</f>
         <v>*WON*[_]C2[_]*</v>
@@ -4059,7 +4466,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C16" s="8" t="str">
         <f t="shared" si="3"/>
         <v>*WON*[_]C3[_]*</v>
@@ -4079,7 +4486,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="17" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C17" s="8" t="str">
         <f t="shared" si="3"/>
         <v>*WON*[_]C4[_]*</v>
@@ -4099,7 +4506,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="18" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C18" s="8" t="str">
         <f t="shared" si="3"/>
         <v>*WON*[_]C5[_]*</v>
@@ -4119,7 +4526,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="19" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C19" s="8" t="str">
         <f t="shared" si="3"/>
         <v>*WON*[_]C6[_]*</v>
@@ -4139,7 +4546,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="20" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C20" s="8" t="str">
         <f t="shared" si="3"/>
         <v>*WON*[_]C7[_]*</v>
@@ -4159,7 +4566,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="21" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C21" s="8" t="str">
         <f t="shared" si="3"/>
         <v>*WON*[_]C8[_]*</v>
@@ -4179,7 +4586,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="22" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C22" s="8" t="str">
         <f t="shared" si="3"/>
         <v>*WON*[_]C9[_]*</v>
@@ -4199,7 +4606,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="23" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C23" s="8" t="str">
         <f t="shared" ref="C23:C31" si="5">"*WOF*[_]"&amp;M23&amp;"[_]*"</f>
         <v>*WOF*[_]C1[_]*</v>
@@ -4225,7 +4632,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="24" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C24" s="8" t="str">
         <f t="shared" si="5"/>
         <v>*WOF*[_]C2[_]*</v>
@@ -4251,7 +4658,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="25" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C25" s="8" t="str">
         <f t="shared" si="5"/>
         <v>*WOF*[_]C3[_]*</v>
@@ -4277,7 +4684,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="26" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C26" s="8" t="str">
         <f t="shared" si="5"/>
         <v>*WOF*[_]C4[_]*</v>
@@ -4303,7 +4710,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="27" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C27" s="8" t="str">
         <f t="shared" si="5"/>
         <v>*WOF*[_]C5[_]*</v>
@@ -4329,7 +4736,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="28" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C28" s="8" t="str">
         <f t="shared" si="5"/>
         <v>*WOF*[_]C6[_]*</v>
@@ -4355,7 +4762,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="29" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C29" s="8" t="str">
         <f t="shared" si="5"/>
         <v>*WOF*[_]C7[_]*</v>
@@ -4381,7 +4788,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="30" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C30" s="8" t="str">
         <f t="shared" si="5"/>
         <v>*WOF*[_]C8[_]*</v>
@@ -4407,7 +4814,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="31" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C31" s="8" t="str">
         <f t="shared" si="5"/>
         <v>*WOF*[_]C9[_]*</v>
@@ -4433,10 +4840,10 @@
         <v>176</v>
       </c>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C34" s="8"/>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C35" s="8"/>
     </row>
   </sheetData>
@@ -4450,24 +4857,24 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -4496,7 +4903,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
         <v>196</v>
       </c>
@@ -4519,7 +4926,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
       <c r="C5" s="5" t="s">
         <v>192</v>
       </c>
@@ -4537,7 +4944,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
       <c r="C6" t="s">
         <v>197</v>
       </c>
@@ -4560,7 +4967,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
       <c r="C7" s="5" t="s">
         <v>193</v>
       </c>
@@ -4577,7 +4984,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
       <c r="C8" t="s">
         <v>194</v>
       </c>
@@ -4594,7 +5001,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
         <v>199</v>
       </c>
@@ -4611,7 +5018,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
         <v>217</v>
       </c>
@@ -4634,7 +5041,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
       <c r="C11" t="s">
         <v>218</v>
       </c>
@@ -4651,7 +5058,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
       <c r="C12" s="5" t="s">
         <v>218</v>
       </c>
@@ -4668,7 +5075,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
         <v>223</v>
       </c>
@@ -4685,7 +5092,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
       <c r="C14" t="s">
         <v>222</v>
       </c>
@@ -4702,7 +5109,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
       <c r="C15" t="s">
         <v>216</v>
       </c>

</xml_diff>

<commit_message>
reporting (adding sources and uses of co2/ccs)
</commit_message>
<xml_diff>
--- a/Sets-IEMM.xlsx
+++ b/Sets-IEMM.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda_models\IEMM_v60_10-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE4A7DBA-C5F5-43B4-8A78-227A1E09F0BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E981D4CB-AB5B-4CB7-AE3F-946A0507DB18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1520" yWindow="1520" windowWidth="14400" windowHeight="8210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="TechSup" sheetId="4" r:id="rId1"/>
-    <sheet name="Comm" sheetId="5" r:id="rId2"/>
-    <sheet name="EFD classification" sheetId="3" r:id="rId3"/>
-    <sheet name="TechTrade" sheetId="6" r:id="rId4"/>
-    <sheet name="Grids" sheetId="7" r:id="rId5"/>
-    <sheet name="SolWin" sheetId="8" r:id="rId6"/>
-    <sheet name="ETL" sheetId="9" r:id="rId7"/>
+    <sheet name="SetsEditor- Proc" sheetId="10" r:id="rId1"/>
+    <sheet name="TechSup" sheetId="4" r:id="rId2"/>
+    <sheet name="Comm" sheetId="5" r:id="rId3"/>
+    <sheet name="EFD classification" sheetId="3" r:id="rId4"/>
+    <sheet name="TechTrade" sheetId="6" r:id="rId5"/>
+    <sheet name="Grids" sheetId="7" r:id="rId6"/>
+    <sheet name="SolWin" sheetId="8" r:id="rId7"/>
+    <sheet name="ETL" sheetId="9" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'EFD classification'!$H$3:$J$78</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TechSup!$F$3:$G$61</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'EFD classification'!$H$3:$J$78</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">TechSup!$F$3:$G$61</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -77,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="335">
   <si>
     <t>Pset_CI</t>
   </si>
@@ -1037,6 +1038,51 @@
   </si>
   <si>
     <t>Or</t>
+  </si>
+  <si>
+    <t>t_pos_andor_forsets</t>
+  </si>
+  <si>
+    <t>t_pos_andor</t>
+  </si>
+  <si>
+    <t>t_neg_andor_forsets</t>
+  </si>
+  <si>
+    <t>t_neg_andor</t>
+  </si>
+  <si>
+    <t>setname</t>
+  </si>
+  <si>
+    <t>setdesc</t>
+  </si>
+  <si>
+    <t>pset_set</t>
+  </si>
+  <si>
+    <t>pset_pn</t>
+  </si>
+  <si>
+    <t>pset_pd</t>
+  </si>
+  <si>
+    <t>pset_co</t>
+  </si>
+  <si>
+    <t>pset_ci</t>
+  </si>
+  <si>
+    <t>And</t>
+  </si>
+  <si>
+    <t>DAC</t>
+  </si>
+  <si>
+    <t>Direct Air Capture</t>
+  </si>
+  <si>
+    <t>SNK_DAC*</t>
   </si>
 </sst>
 </file>
@@ -1525,11 +1571,90 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6893ED32-2DE5-4115-A4E9-926B8F20B6FA}">
+  <dimension ref="A1:K3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B2" t="s">
+        <v>321</v>
+      </c>
+      <c r="C2" t="s">
+        <v>322</v>
+      </c>
+      <c r="D2" t="s">
+        <v>323</v>
+      </c>
+      <c r="E2" t="s">
+        <v>324</v>
+      </c>
+      <c r="F2" t="s">
+        <v>325</v>
+      </c>
+      <c r="G2" t="s">
+        <v>326</v>
+      </c>
+      <c r="H2" t="s">
+        <v>327</v>
+      </c>
+      <c r="I2" t="s">
+        <v>328</v>
+      </c>
+      <c r="J2" t="s">
+        <v>329</v>
+      </c>
+      <c r="K2" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>331</v>
+      </c>
+      <c r="B3" t="s">
+        <v>331</v>
+      </c>
+      <c r="C3" t="s">
+        <v>331</v>
+      </c>
+      <c r="D3" t="s">
+        <v>331</v>
+      </c>
+      <c r="E3" t="s">
+        <v>332</v>
+      </c>
+      <c r="F3" t="s">
+        <v>333</v>
+      </c>
+      <c r="G3" t="s">
+        <v>266</v>
+      </c>
+      <c r="H3" t="s">
+        <v>334</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B2:J86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D79" sqref="D79"/>
     </sheetView>
@@ -3066,7 +3191,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B2:G11"/>
@@ -3247,7 +3372,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B2:O58"/>
@@ -4144,7 +4269,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="B2:J3"/>
@@ -4192,7 +4317,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B2:J8"/>
   <sheetViews>
@@ -4318,7 +4443,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B2:M35"/>
   <sheetViews>
@@ -5001,7 +5126,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="B2:J15"/>
   <sheetViews>

</xml_diff>